<commit_message>
Seperate note render and game playing code
</commit_message>
<xml_diff>
--- a/Utility/xlsFiles/아기 알파카는 오늘도 꿈을 꾸고 있어요.xlsx
+++ b/Utility/xlsFiles/아기 알파카는 오늘도 꿈을 꾸고 있어요.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20383"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28F6719F-4481-44B3-BC31-6789E36D6AFA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A31ED98-951C-4536-B79B-7D95551BA7E3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6025,8 +6025,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E07BD68-F4D3-493E-B579-B52A0BB22360}">
   <dimension ref="A1:K380"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="O21" sqref="O21"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -9914,7 +9914,7 @@
     <mergeCell ref="J1:K1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="J2:J88">
+  <conditionalFormatting sqref="J2:J116">
     <cfRule type="expression" dxfId="50" priority="10">
       <formula>IF(AND(EXACT($A2,"w"), (OR(EXACT($B2,"l"), EXACT($B2,"b")))), TRUE, FALSE)</formula>
     </cfRule>
@@ -9937,7 +9937,7 @@
       <formula>IF(AND(EXACT($A2,"r"), (OR(EXACT($B2,"l"), EXACT($B2,"b")))), TRUE, FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K3:K72">
+  <conditionalFormatting sqref="K3:K116">
     <cfRule type="expression" dxfId="43" priority="11">
       <formula>IF(AND(EXACT($A3,"w"), EXACT($B3,"r")), TRUE, FALSE)</formula>
     </cfRule>
@@ -9960,17 +9960,17 @@
       <formula>IF(AND(EXACT($A3,"r"), EXACT($B3,"r")), TRUE, FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J59 K2:K84">
+  <conditionalFormatting sqref="J2:K116">
     <cfRule type="expression" dxfId="36" priority="58">
       <formula>OR(EXACT($B2,"r"), EXACT($B2,"b"))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K3:K64">
+  <conditionalFormatting sqref="K3:K116">
     <cfRule type="expression" dxfId="35" priority="9">
       <formula>EXACT($B3,"l")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K84">
+  <conditionalFormatting sqref="K2:K116">
     <cfRule type="expression" dxfId="34" priority="1">
       <formula>IF(AND(EXACT($A2,"w"), (OR(EXACT($B2,"r"), EXACT($B2,"b")))), TRUE, FALSE)</formula>
     </cfRule>

</xml_diff>